<commit_message>
Slight changes and bug fixes
</commit_message>
<xml_diff>
--- a/data/Football Data Dump.xlsx
+++ b/data/Football Data Dump.xlsx
@@ -583,31 +583,31 @@
         <v>1.0</v>
       </c>
       <c r="AL2" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AM2" s="1">
         <v>1.0</v>
       </c>
       <c r="AN2" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AO2" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AP2" s="1">
         <v>1.0</v>
       </c>
       <c r="AQ2" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AR2" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AS2" s="1">
         <v>1.0</v>
       </c>
       <c r="AT2" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="3">
@@ -723,31 +723,31 @@
         <v>1.0</v>
       </c>
       <c r="AL3" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AM3" s="1">
         <v>1.0</v>
       </c>
       <c r="AN3" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AO3" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AP3" s="1">
         <v>1.0</v>
       </c>
       <c r="AQ3" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AR3" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AS3" s="1">
         <v>1.0</v>
       </c>
       <c r="AT3" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="4">
@@ -863,31 +863,31 @@
         <v>1.0</v>
       </c>
       <c r="AL4" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AM4" s="1">
         <v>1.0</v>
       </c>
       <c r="AN4" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AO4" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AP4" s="1">
         <v>1.0</v>
       </c>
       <c r="AQ4" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AR4" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AS4" s="1">
         <v>1.0</v>
       </c>
       <c r="AT4" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="5">
@@ -1003,31 +1003,31 @@
         <v>1.0</v>
       </c>
       <c r="AL5" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AM5" s="1">
         <v>1.0</v>
       </c>
       <c r="AN5" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AO5" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AP5" s="1">
         <v>1.0</v>
       </c>
       <c r="AQ5" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AR5" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AS5" s="1">
         <v>1.0</v>
       </c>
       <c r="AT5" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="6">
@@ -1143,31 +1143,31 @@
         <v>1.0</v>
       </c>
       <c r="AL6" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AM6" s="1">
         <v>1.0</v>
       </c>
       <c r="AN6" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AO6" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AP6" s="1">
         <v>1.0</v>
       </c>
       <c r="AQ6" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AR6" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AS6" s="1">
         <v>1.0</v>
       </c>
       <c r="AT6" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="7">
@@ -1283,31 +1283,31 @@
         <v>1.0</v>
       </c>
       <c r="AL7" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AM7" s="1">
         <v>1.0</v>
       </c>
       <c r="AN7" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AO7" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AP7" s="1">
         <v>1.0</v>
       </c>
       <c r="AQ7" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AR7" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AS7" s="1">
         <v>1.0</v>
       </c>
       <c r="AT7" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="8">
@@ -1423,31 +1423,31 @@
         <v>1.0</v>
       </c>
       <c r="AL8" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AM8" s="1">
         <v>1.0</v>
       </c>
       <c r="AN8" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AO8" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AP8" s="1">
         <v>1.0</v>
       </c>
       <c r="AQ8" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AR8" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AS8" s="1">
         <v>1.0</v>
       </c>
       <c r="AT8" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="9">
@@ -1563,31 +1563,31 @@
         <v>1.0</v>
       </c>
       <c r="AL9" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AM9" s="1">
         <v>1.0</v>
       </c>
       <c r="AN9" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AO9" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AP9" s="1">
         <v>1.0</v>
       </c>
       <c r="AQ9" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AR9" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AS9" s="1">
         <v>1.0</v>
       </c>
       <c r="AT9" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="10">
@@ -1703,31 +1703,31 @@
         <v>1.0</v>
       </c>
       <c r="AL10" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AM10" s="1">
         <v>1.0</v>
       </c>
       <c r="AN10" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AO10" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AP10" s="1">
         <v>1.0</v>
       </c>
       <c r="AQ10" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AR10" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AS10" s="1">
         <v>1.0</v>
       </c>
       <c r="AT10" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="11">
@@ -1843,31 +1843,31 @@
         <v>1.0</v>
       </c>
       <c r="AL11" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AM11" s="1">
         <v>1.0</v>
       </c>
       <c r="AN11" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AO11" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AP11" s="1">
         <v>1.0</v>
       </c>
       <c r="AQ11" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AR11" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AS11" s="1">
         <v>1.0</v>
       </c>
       <c r="AT11" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="12">
@@ -1983,31 +1983,31 @@
         <v>1.0</v>
       </c>
       <c r="AL12" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AM12" s="1">
         <v>1.0</v>
       </c>
       <c r="AN12" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AO12" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AP12" s="1">
         <v>1.0</v>
       </c>
       <c r="AQ12" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AR12" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AS12" s="1">
         <v>1.0</v>
       </c>
       <c r="AT12" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="13">
@@ -2123,31 +2123,31 @@
         <v>1.0</v>
       </c>
       <c r="AL13" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AM13" s="1">
         <v>1.0</v>
       </c>
       <c r="AN13" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AO13" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AP13" s="1">
         <v>1.0</v>
       </c>
       <c r="AQ13" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AR13" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AS13" s="1">
         <v>1.0</v>
       </c>
       <c r="AT13" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="14">
@@ -2263,31 +2263,31 @@
         <v>1.0</v>
       </c>
       <c r="AL14" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AM14" s="1">
         <v>1.0</v>
       </c>
       <c r="AN14" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AO14" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AP14" s="1">
         <v>1.0</v>
       </c>
       <c r="AQ14" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AR14" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AS14" s="1">
         <v>1.0</v>
       </c>
       <c r="AT14" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="15">
@@ -2403,31 +2403,31 @@
         <v>1.0</v>
       </c>
       <c r="AL15" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AM15" s="1">
         <v>1.0</v>
       </c>
       <c r="AN15" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AO15" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AP15" s="1">
         <v>1.0</v>
       </c>
       <c r="AQ15" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AR15" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AS15" s="1">
         <v>1.0</v>
       </c>
       <c r="AT15" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="16">
@@ -2543,31 +2543,31 @@
         <v>1.0</v>
       </c>
       <c r="AL16" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AM16" s="1">
         <v>1.0</v>
       </c>
       <c r="AN16" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AO16" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AP16" s="1">
         <v>1.0</v>
       </c>
       <c r="AQ16" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AR16" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AS16" s="1">
         <v>1.0</v>
       </c>
       <c r="AT16" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="17">
@@ -2632,49 +2632,49 @@
         <v>1.0</v>
       </c>
       <c r="U17" s="1">
-        <v>1.0</v>
+        <v>6.0</v>
       </c>
       <c r="V17" s="8">
         <v>1.0</v>
       </c>
-      <c r="W17" s="7">
-        <v>1.0</v>
+      <c r="W17" s="1">
+        <v>2.0</v>
       </c>
       <c r="X17" s="1">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
       <c r="Y17" s="8">
-        <v>1.0</v>
-      </c>
-      <c r="Z17" s="7">
-        <v>1.0</v>
+        <v>6.0</v>
+      </c>
+      <c r="Z17" s="1">
+        <v>6.0</v>
       </c>
       <c r="AA17" s="1">
-        <v>1.0</v>
+        <v>7.0</v>
       </c>
       <c r="AB17" s="8">
-        <v>1.0</v>
-      </c>
-      <c r="AC17" s="7">
-        <v>1.0</v>
+        <v>8.0</v>
+      </c>
+      <c r="AC17" s="1">
+        <v>6.0</v>
       </c>
       <c r="AD17" s="1">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="AE17" s="8">
-        <v>1.0</v>
-      </c>
-      <c r="AF17" s="7">
-        <v>1.0</v>
+        <v>6.0</v>
+      </c>
+      <c r="AF17" s="1">
+        <v>3.0</v>
       </c>
       <c r="AG17" s="1">
-        <v>1.0</v>
+        <v>6.0</v>
       </c>
       <c r="AH17" s="8">
-        <v>1.0</v>
-      </c>
-      <c r="AI17" s="7">
-        <v>1.0</v>
+        <v>2.0</v>
+      </c>
+      <c r="AI17" s="1">
+        <v>6.0</v>
       </c>
       <c r="AJ17" s="1">
         <v>1.0</v>
@@ -2683,31 +2683,31 @@
         <v>1.0</v>
       </c>
       <c r="AL17" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AM17" s="1">
         <v>1.0</v>
       </c>
       <c r="AN17" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AO17" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AP17" s="1">
         <v>1.0</v>
       </c>
       <c r="AQ17" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AR17" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AS17" s="1">
         <v>1.0</v>
       </c>
       <c r="AT17" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="18">
@@ -2772,49 +2772,49 @@
         <v>1.0</v>
       </c>
       <c r="U18" s="1">
-        <v>1.0</v>
+        <v>6.0</v>
       </c>
       <c r="V18" s="8">
         <v>1.0</v>
       </c>
-      <c r="W18" s="7">
-        <v>1.0</v>
+      <c r="W18" s="1">
+        <v>2.0</v>
       </c>
       <c r="X18" s="1">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
       <c r="Y18" s="8">
-        <v>1.0</v>
-      </c>
-      <c r="Z18" s="7">
-        <v>1.0</v>
+        <v>6.0</v>
+      </c>
+      <c r="Z18" s="1">
+        <v>6.0</v>
       </c>
       <c r="AA18" s="1">
-        <v>1.0</v>
+        <v>7.0</v>
       </c>
       <c r="AB18" s="8">
-        <v>1.0</v>
-      </c>
-      <c r="AC18" s="7">
-        <v>1.0</v>
+        <v>8.0</v>
+      </c>
+      <c r="AC18" s="1">
+        <v>6.0</v>
       </c>
       <c r="AD18" s="1">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="AE18" s="8">
-        <v>1.0</v>
-      </c>
-      <c r="AF18" s="7">
-        <v>1.0</v>
+        <v>6.0</v>
+      </c>
+      <c r="AF18" s="1">
+        <v>3.0</v>
       </c>
       <c r="AG18" s="1">
-        <v>1.0</v>
+        <v>6.0</v>
       </c>
       <c r="AH18" s="8">
-        <v>1.0</v>
-      </c>
-      <c r="AI18" s="7">
-        <v>1.0</v>
+        <v>2.0</v>
+      </c>
+      <c r="AI18" s="1">
+        <v>6.0</v>
       </c>
       <c r="AJ18" s="1">
         <v>1.0</v>
@@ -2823,31 +2823,31 @@
         <v>1.0</v>
       </c>
       <c r="AL18" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AM18" s="1">
         <v>1.0</v>
       </c>
       <c r="AN18" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AO18" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AP18" s="1">
         <v>1.0</v>
       </c>
       <c r="AQ18" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AR18" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AS18" s="1">
         <v>1.0</v>
       </c>
       <c r="AT18" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="19">
@@ -2912,49 +2912,49 @@
         <v>1.0</v>
       </c>
       <c r="U19" s="1">
-        <v>1.0</v>
+        <v>6.0</v>
       </c>
       <c r="V19" s="8">
         <v>1.0</v>
       </c>
-      <c r="W19" s="7">
-        <v>1.0</v>
+      <c r="W19" s="1">
+        <v>2.0</v>
       </c>
       <c r="X19" s="1">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
       <c r="Y19" s="8">
-        <v>1.0</v>
-      </c>
-      <c r="Z19" s="7">
-        <v>1.0</v>
+        <v>6.0</v>
+      </c>
+      <c r="Z19" s="1">
+        <v>6.0</v>
       </c>
       <c r="AA19" s="1">
-        <v>1.0</v>
+        <v>7.0</v>
       </c>
       <c r="AB19" s="8">
-        <v>1.0</v>
-      </c>
-      <c r="AC19" s="7">
-        <v>1.0</v>
+        <v>8.0</v>
+      </c>
+      <c r="AC19" s="1">
+        <v>6.0</v>
       </c>
       <c r="AD19" s="1">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="AE19" s="8">
-        <v>1.0</v>
-      </c>
-      <c r="AF19" s="7">
-        <v>1.0</v>
+        <v>6.0</v>
+      </c>
+      <c r="AF19" s="1">
+        <v>3.0</v>
       </c>
       <c r="AG19" s="1">
-        <v>1.0</v>
+        <v>6.0</v>
       </c>
       <c r="AH19" s="8">
-        <v>1.0</v>
-      </c>
-      <c r="AI19" s="7">
-        <v>1.0</v>
+        <v>2.0</v>
+      </c>
+      <c r="AI19" s="1">
+        <v>6.0</v>
       </c>
       <c r="AJ19" s="1">
         <v>1.0</v>
@@ -2963,31 +2963,31 @@
         <v>1.0</v>
       </c>
       <c r="AL19" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AM19" s="1">
         <v>1.0</v>
       </c>
       <c r="AN19" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AO19" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AP19" s="1">
         <v>1.0</v>
       </c>
       <c r="AQ19" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AR19" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AS19" s="1">
         <v>1.0</v>
       </c>
       <c r="AT19" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="20">
@@ -3052,49 +3052,49 @@
         <v>1.0</v>
       </c>
       <c r="U20" s="1">
-        <v>1.0</v>
+        <v>6.0</v>
       </c>
       <c r="V20" s="8">
         <v>1.0</v>
       </c>
-      <c r="W20" s="7">
-        <v>1.0</v>
+      <c r="W20" s="1">
+        <v>2.0</v>
       </c>
       <c r="X20" s="1">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
       <c r="Y20" s="8">
-        <v>1.0</v>
-      </c>
-      <c r="Z20" s="7">
-        <v>1.0</v>
+        <v>6.0</v>
+      </c>
+      <c r="Z20" s="1">
+        <v>6.0</v>
       </c>
       <c r="AA20" s="1">
-        <v>1.0</v>
+        <v>7.0</v>
       </c>
       <c r="AB20" s="8">
-        <v>1.0</v>
-      </c>
-      <c r="AC20" s="7">
-        <v>1.0</v>
+        <v>8.0</v>
+      </c>
+      <c r="AC20" s="1">
+        <v>6.0</v>
       </c>
       <c r="AD20" s="1">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="AE20" s="8">
-        <v>1.0</v>
-      </c>
-      <c r="AF20" s="7">
-        <v>1.0</v>
+        <v>6.0</v>
+      </c>
+      <c r="AF20" s="1">
+        <v>3.0</v>
       </c>
       <c r="AG20" s="1">
-        <v>1.0</v>
+        <v>6.0</v>
       </c>
       <c r="AH20" s="8">
-        <v>1.0</v>
-      </c>
-      <c r="AI20" s="7">
-        <v>1.0</v>
+        <v>2.0</v>
+      </c>
+      <c r="AI20" s="1">
+        <v>6.0</v>
       </c>
       <c r="AJ20" s="1">
         <v>1.0</v>
@@ -3103,31 +3103,31 @@
         <v>1.0</v>
       </c>
       <c r="AL20" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AM20" s="1">
         <v>1.0</v>
       </c>
       <c r="AN20" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AO20" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AP20" s="1">
         <v>1.0</v>
       </c>
       <c r="AQ20" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AR20" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AS20" s="1">
         <v>1.0</v>
       </c>
       <c r="AT20" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="21">
@@ -3192,49 +3192,49 @@
         <v>1.0</v>
       </c>
       <c r="U21" s="1">
-        <v>1.0</v>
+        <v>6.0</v>
       </c>
       <c r="V21" s="8">
         <v>1.0</v>
       </c>
-      <c r="W21" s="7">
-        <v>1.0</v>
+      <c r="W21" s="1">
+        <v>2.0</v>
       </c>
       <c r="X21" s="1">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
       <c r="Y21" s="8">
-        <v>1.0</v>
-      </c>
-      <c r="Z21" s="7">
-        <v>1.0</v>
+        <v>6.0</v>
+      </c>
+      <c r="Z21" s="1">
+        <v>6.0</v>
       </c>
       <c r="AA21" s="1">
-        <v>1.0</v>
+        <v>7.0</v>
       </c>
       <c r="AB21" s="8">
-        <v>1.0</v>
-      </c>
-      <c r="AC21" s="7">
-        <v>1.0</v>
+        <v>8.0</v>
+      </c>
+      <c r="AC21" s="1">
+        <v>6.0</v>
       </c>
       <c r="AD21" s="1">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="AE21" s="8">
-        <v>1.0</v>
-      </c>
-      <c r="AF21" s="7">
-        <v>1.0</v>
+        <v>6.0</v>
+      </c>
+      <c r="AF21" s="1">
+        <v>3.0</v>
       </c>
       <c r="AG21" s="1">
-        <v>1.0</v>
+        <v>6.0</v>
       </c>
       <c r="AH21" s="8">
-        <v>1.0</v>
-      </c>
-      <c r="AI21" s="7">
-        <v>1.0</v>
+        <v>2.0</v>
+      </c>
+      <c r="AI21" s="1">
+        <v>6.0</v>
       </c>
       <c r="AJ21" s="1">
         <v>1.0</v>
@@ -3243,31 +3243,31 @@
         <v>1.0</v>
       </c>
       <c r="AL21" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AM21" s="1">
         <v>1.0</v>
       </c>
       <c r="AN21" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AO21" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AP21" s="1">
         <v>1.0</v>
       </c>
       <c r="AQ21" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AR21" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AS21" s="1">
         <v>1.0</v>
       </c>
       <c r="AT21" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="22">
@@ -3332,49 +3332,49 @@
         <v>1.0</v>
       </c>
       <c r="U22" s="1">
-        <v>1.0</v>
+        <v>6.0</v>
       </c>
       <c r="V22" s="8">
         <v>1.0</v>
       </c>
-      <c r="W22" s="7">
-        <v>1.0</v>
+      <c r="W22" s="1">
+        <v>2.0</v>
       </c>
       <c r="X22" s="1">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
       <c r="Y22" s="8">
-        <v>1.0</v>
-      </c>
-      <c r="Z22" s="7">
-        <v>1.0</v>
+        <v>6.0</v>
+      </c>
+      <c r="Z22" s="1">
+        <v>6.0</v>
       </c>
       <c r="AA22" s="1">
-        <v>1.0</v>
+        <v>7.0</v>
       </c>
       <c r="AB22" s="8">
-        <v>1.0</v>
-      </c>
-      <c r="AC22" s="7">
-        <v>1.0</v>
+        <v>8.0</v>
+      </c>
+      <c r="AC22" s="1">
+        <v>6.0</v>
       </c>
       <c r="AD22" s="1">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="AE22" s="8">
-        <v>1.0</v>
-      </c>
-      <c r="AF22" s="7">
-        <v>1.0</v>
+        <v>6.0</v>
+      </c>
+      <c r="AF22" s="1">
+        <v>3.0</v>
       </c>
       <c r="AG22" s="1">
-        <v>1.0</v>
+        <v>6.0</v>
       </c>
       <c r="AH22" s="8">
-        <v>1.0</v>
-      </c>
-      <c r="AI22" s="7">
-        <v>1.0</v>
+        <v>2.0</v>
+      </c>
+      <c r="AI22" s="1">
+        <v>6.0</v>
       </c>
       <c r="AJ22" s="1">
         <v>1.0</v>
@@ -3383,31 +3383,31 @@
         <v>1.0</v>
       </c>
       <c r="AL22" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AM22" s="1">
         <v>1.0</v>
       </c>
       <c r="AN22" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AO22" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AP22" s="1">
         <v>1.0</v>
       </c>
       <c r="AQ22" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AR22" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AS22" s="1">
         <v>1.0</v>
       </c>
       <c r="AT22" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="23">
@@ -3472,49 +3472,49 @@
         <v>1.0</v>
       </c>
       <c r="U23" s="1">
-        <v>1.0</v>
+        <v>6.0</v>
       </c>
       <c r="V23" s="8">
         <v>1.0</v>
       </c>
-      <c r="W23" s="7">
-        <v>1.0</v>
+      <c r="W23" s="1">
+        <v>2.0</v>
       </c>
       <c r="X23" s="1">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
       <c r="Y23" s="8">
-        <v>1.0</v>
-      </c>
-      <c r="Z23" s="7">
-        <v>1.0</v>
+        <v>6.0</v>
+      </c>
+      <c r="Z23" s="1">
+        <v>6.0</v>
       </c>
       <c r="AA23" s="1">
-        <v>1.0</v>
+        <v>7.0</v>
       </c>
       <c r="AB23" s="8">
-        <v>1.0</v>
-      </c>
-      <c r="AC23" s="7">
-        <v>1.0</v>
+        <v>8.0</v>
+      </c>
+      <c r="AC23" s="1">
+        <v>6.0</v>
       </c>
       <c r="AD23" s="1">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="AE23" s="8">
-        <v>1.0</v>
-      </c>
-      <c r="AF23" s="7">
-        <v>1.0</v>
+        <v>6.0</v>
+      </c>
+      <c r="AF23" s="1">
+        <v>3.0</v>
       </c>
       <c r="AG23" s="1">
-        <v>1.0</v>
+        <v>6.0</v>
       </c>
       <c r="AH23" s="8">
-        <v>1.0</v>
-      </c>
-      <c r="AI23" s="7">
-        <v>1.0</v>
+        <v>2.0</v>
+      </c>
+      <c r="AI23" s="1">
+        <v>6.0</v>
       </c>
       <c r="AJ23" s="1">
         <v>1.0</v>
@@ -3523,31 +3523,31 @@
         <v>1.0</v>
       </c>
       <c r="AL23" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AM23" s="1">
         <v>1.0</v>
       </c>
       <c r="AN23" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AO23" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AP23" s="1">
         <v>1.0</v>
       </c>
       <c r="AQ23" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AR23" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AS23" s="1">
         <v>1.0</v>
       </c>
       <c r="AT23" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="24">
@@ -3663,31 +3663,31 @@
         <v>1.0</v>
       </c>
       <c r="AL24" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AM24" s="1">
         <v>1.0</v>
       </c>
       <c r="AN24" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AO24" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AP24" s="1">
         <v>1.0</v>
       </c>
       <c r="AQ24" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AR24" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AS24" s="1">
         <v>1.0</v>
       </c>
       <c r="AT24" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="25">
@@ -3803,31 +3803,31 @@
         <v>1.0</v>
       </c>
       <c r="AL25" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AM25" s="1">
         <v>1.0</v>
       </c>
       <c r="AN25" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AO25" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AP25" s="1">
         <v>1.0</v>
       </c>
       <c r="AQ25" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AR25" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AS25" s="1">
         <v>1.0</v>
       </c>
       <c r="AT25" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="26">
@@ -3943,31 +3943,31 @@
         <v>1.0</v>
       </c>
       <c r="AL26" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AM26" s="1">
         <v>1.0</v>
       </c>
       <c r="AN26" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AO26" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AP26" s="1">
         <v>1.0</v>
       </c>
       <c r="AQ26" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AR26" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AS26" s="1">
         <v>1.0</v>
       </c>
       <c r="AT26" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="27">
@@ -4083,31 +4083,31 @@
         <v>1.0</v>
       </c>
       <c r="AL27" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AM27" s="1">
         <v>1.0</v>
       </c>
       <c r="AN27" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AO27" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AP27" s="1">
         <v>1.0</v>
       </c>
       <c r="AQ27" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AR27" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AS27" s="1">
         <v>1.0</v>
       </c>
       <c r="AT27" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="28">
@@ -4223,31 +4223,31 @@
         <v>1.0</v>
       </c>
       <c r="AL28" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AM28" s="1">
         <v>1.0</v>
       </c>
       <c r="AN28" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AO28" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AP28" s="1">
         <v>1.0</v>
       </c>
       <c r="AQ28" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AR28" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AS28" s="1">
         <v>1.0</v>
       </c>
       <c r="AT28" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="29">
@@ -4363,31 +4363,31 @@
         <v>1.0</v>
       </c>
       <c r="AL29" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AM29" s="1">
         <v>1.0</v>
       </c>
       <c r="AN29" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AO29" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AP29" s="1">
         <v>1.0</v>
       </c>
       <c r="AQ29" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AR29" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AS29" s="1">
         <v>1.0</v>
       </c>
       <c r="AT29" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="30">
@@ -4503,31 +4503,31 @@
         <v>1.0</v>
       </c>
       <c r="AL30" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AM30" s="1">
         <v>1.0</v>
       </c>
       <c r="AN30" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AO30" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AP30" s="1">
         <v>1.0</v>
       </c>
       <c r="AQ30" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AR30" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AS30" s="1">
         <v>1.0</v>
       </c>
       <c r="AT30" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="31">
@@ -4643,31 +4643,31 @@
         <v>1.0</v>
       </c>
       <c r="AL31" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AM31" s="1">
         <v>1.0</v>
       </c>
       <c r="AN31" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AO31" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AP31" s="1">
         <v>1.0</v>
       </c>
       <c r="AQ31" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AR31" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AS31" s="1">
         <v>1.0</v>
       </c>
       <c r="AT31" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="32">
@@ -4783,31 +4783,31 @@
         <v>1.0</v>
       </c>
       <c r="AL32" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AM32" s="1">
         <v>1.0</v>
       </c>
       <c r="AN32" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AO32" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AP32" s="1">
         <v>1.0</v>
       </c>
       <c r="AQ32" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AR32" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AS32" s="1">
         <v>1.0</v>
       </c>
       <c r="AT32" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="33">
@@ -4923,31 +4923,31 @@
         <v>1.0</v>
       </c>
       <c r="AL33" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AM33" s="1">
         <v>1.0</v>
       </c>
       <c r="AN33" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AO33" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AP33" s="1">
         <v>1.0</v>
       </c>
       <c r="AQ33" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AR33" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AS33" s="1">
         <v>1.0</v>
       </c>
       <c r="AT33" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="34">
@@ -5063,31 +5063,31 @@
         <v>1.0</v>
       </c>
       <c r="AL34" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AM34" s="1">
         <v>1.0</v>
       </c>
       <c r="AN34" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AO34" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AP34" s="1">
         <v>1.0</v>
       </c>
       <c r="AQ34" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AR34" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AS34" s="1">
         <v>1.0</v>
       </c>
       <c r="AT34" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="35">
@@ -5203,31 +5203,31 @@
         <v>1.0</v>
       </c>
       <c r="AL35" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AM35" s="1">
         <v>1.0</v>
       </c>
       <c r="AN35" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AO35" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AP35" s="1">
         <v>1.0</v>
       </c>
       <c r="AQ35" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AR35" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AS35" s="1">
         <v>1.0</v>
       </c>
       <c r="AT35" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="36">
@@ -5343,31 +5343,31 @@
         <v>1.0</v>
       </c>
       <c r="AL36" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AM36" s="1">
         <v>1.0</v>
       </c>
       <c r="AN36" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AO36" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AP36" s="1">
         <v>1.0</v>
       </c>
       <c r="AQ36" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AR36" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AS36" s="1">
         <v>1.0</v>
       </c>
       <c r="AT36" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="37">
@@ -5483,31 +5483,31 @@
         <v>1.0</v>
       </c>
       <c r="AL37" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AM37" s="1">
         <v>1.0</v>
       </c>
       <c r="AN37" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AO37" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AP37" s="1">
         <v>1.0</v>
       </c>
       <c r="AQ37" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AR37" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AS37" s="1">
         <v>1.0</v>
       </c>
       <c r="AT37" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="38">
@@ -5623,31 +5623,31 @@
         <v>1.0</v>
       </c>
       <c r="AL38" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AM38" s="1">
         <v>1.0</v>
       </c>
       <c r="AN38" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AO38" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AP38" s="1">
         <v>1.0</v>
       </c>
       <c r="AQ38" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AR38" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AS38" s="1">
         <v>1.0</v>
       </c>
       <c r="AT38" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="39">
@@ -5763,31 +5763,31 @@
         <v>1.0</v>
       </c>
       <c r="AL39" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AM39" s="1">
         <v>1.0</v>
       </c>
       <c r="AN39" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AO39" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AP39" s="1">
         <v>1.0</v>
       </c>
       <c r="AQ39" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AR39" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AS39" s="1">
         <v>1.0</v>
       </c>
       <c r="AT39" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="40">
@@ -5903,31 +5903,31 @@
         <v>1.0</v>
       </c>
       <c r="AL40" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AM40" s="1">
         <v>1.0</v>
       </c>
       <c r="AN40" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AO40" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AP40" s="1">
         <v>1.0</v>
       </c>
       <c r="AQ40" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AR40" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AS40" s="1">
         <v>1.0</v>
       </c>
       <c r="AT40" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="41">
@@ -6043,31 +6043,31 @@
         <v>1.0</v>
       </c>
       <c r="AL41" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AM41" s="1">
         <v>1.0</v>
       </c>
       <c r="AN41" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AO41" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AP41" s="1">
         <v>1.0</v>
       </c>
       <c r="AQ41" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AR41" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AS41" s="1">
         <v>1.0</v>
       </c>
       <c r="AT41" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="42">
@@ -6183,31 +6183,31 @@
         <v>1.0</v>
       </c>
       <c r="AL42" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AM42" s="1">
         <v>1.0</v>
       </c>
       <c r="AN42" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AO42" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AP42" s="1">
         <v>1.0</v>
       </c>
       <c r="AQ42" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AR42" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AS42" s="1">
         <v>1.0</v>
       </c>
       <c r="AT42" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="43">
@@ -6323,31 +6323,31 @@
         <v>1.0</v>
       </c>
       <c r="AL43" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AM43" s="1">
         <v>1.0</v>
       </c>
       <c r="AN43" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AO43" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AP43" s="1">
         <v>1.0</v>
       </c>
       <c r="AQ43" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AR43" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AS43" s="1">
         <v>1.0</v>
       </c>
       <c r="AT43" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="44">
@@ -6463,31 +6463,31 @@
         <v>1.0</v>
       </c>
       <c r="AL44" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AM44" s="1">
         <v>1.0</v>
       </c>
       <c r="AN44" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AO44" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AP44" s="1">
         <v>1.0</v>
       </c>
       <c r="AQ44" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AR44" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AS44" s="1">
         <v>1.0</v>
       </c>
       <c r="AT44" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="45">
@@ -6603,31 +6603,31 @@
         <v>1.0</v>
       </c>
       <c r="AL45" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AM45" s="1">
         <v>1.0</v>
       </c>
       <c r="AN45" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AO45" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AP45" s="1">
         <v>1.0</v>
       </c>
       <c r="AQ45" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AR45" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AS45" s="1">
         <v>1.0</v>
       </c>
       <c r="AT45" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="46">
@@ -6743,31 +6743,31 @@
         <v>1.0</v>
       </c>
       <c r="AL46" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AM46" s="1">
         <v>1.0</v>
       </c>
       <c r="AN46" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AO46" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AP46" s="1">
         <v>1.0</v>
       </c>
       <c r="AQ46" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AR46" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AS46" s="1">
         <v>1.0</v>
       </c>
       <c r="AT46" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="47">
@@ -6883,31 +6883,31 @@
         <v>1.0</v>
       </c>
       <c r="AL47" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AM47" s="1">
         <v>1.0</v>
       </c>
       <c r="AN47" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AO47" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AP47" s="1">
         <v>1.0</v>
       </c>
       <c r="AQ47" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AR47" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AS47" s="1">
         <v>1.0</v>
       </c>
       <c r="AT47" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="48">
@@ -7023,31 +7023,31 @@
         <v>1.0</v>
       </c>
       <c r="AL48" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AM48" s="1">
         <v>1.0</v>
       </c>
       <c r="AN48" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AO48" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AP48" s="1">
         <v>1.0</v>
       </c>
       <c r="AQ48" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AR48" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AS48" s="1">
         <v>1.0</v>
       </c>
       <c r="AT48" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="49">
@@ -7163,31 +7163,31 @@
         <v>1.0</v>
       </c>
       <c r="AL49" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AM49" s="1">
         <v>1.0</v>
       </c>
       <c r="AN49" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AO49" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AP49" s="1">
         <v>1.0</v>
       </c>
       <c r="AQ49" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AR49" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AS49" s="1">
         <v>1.0</v>
       </c>
       <c r="AT49" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="50">
@@ -7303,31 +7303,31 @@
         <v>1.0</v>
       </c>
       <c r="AL50" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AM50" s="1">
         <v>1.0</v>
       </c>
       <c r="AN50" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AO50" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AP50" s="1">
         <v>1.0</v>
       </c>
       <c r="AQ50" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AR50" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AS50" s="1">
         <v>1.0</v>
       </c>
       <c r="AT50" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="51">
@@ -7443,31 +7443,31 @@
         <v>1.0</v>
       </c>
       <c r="AL51" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AM51" s="1">
         <v>1.0</v>
       </c>
       <c r="AN51" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AO51" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AP51" s="1">
         <v>1.0</v>
       </c>
       <c r="AQ51" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AR51" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AS51" s="1">
         <v>1.0</v>
       </c>
       <c r="AT51" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="52">
@@ -7583,31 +7583,31 @@
         <v>1.0</v>
       </c>
       <c r="AL52" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AM52" s="1">
         <v>1.0</v>
       </c>
       <c r="AN52" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AO52" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AP52" s="1">
         <v>1.0</v>
       </c>
       <c r="AQ52" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AR52" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AS52" s="1">
         <v>1.0</v>
       </c>
       <c r="AT52" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="53">
@@ -7723,31 +7723,31 @@
         <v>1.0</v>
       </c>
       <c r="AL53" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AM53" s="1">
         <v>1.0</v>
       </c>
       <c r="AN53" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AO53" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AP53" s="1">
         <v>1.0</v>
       </c>
       <c r="AQ53" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AR53" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AS53" s="1">
         <v>1.0</v>
       </c>
       <c r="AT53" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="54">
@@ -7863,31 +7863,31 @@
         <v>1.0</v>
       </c>
       <c r="AL54" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AM54" s="1">
         <v>1.0</v>
       </c>
       <c r="AN54" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AO54" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AP54" s="1">
         <v>1.0</v>
       </c>
       <c r="AQ54" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AR54" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AS54" s="1">
         <v>1.0</v>
       </c>
       <c r="AT54" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="55">
@@ -8003,31 +8003,31 @@
         <v>1.0</v>
       </c>
       <c r="AL55" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AM55" s="1">
         <v>1.0</v>
       </c>
       <c r="AN55" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AO55" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AP55" s="1">
         <v>1.0</v>
       </c>
       <c r="AQ55" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AR55" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AS55" s="1">
         <v>1.0</v>
       </c>
       <c r="AT55" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="56">
@@ -8143,31 +8143,31 @@
         <v>1.0</v>
       </c>
       <c r="AL56" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AM56" s="1">
         <v>1.0</v>
       </c>
       <c r="AN56" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AO56" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AP56" s="1">
         <v>1.0</v>
       </c>
       <c r="AQ56" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AR56" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AS56" s="1">
         <v>1.0</v>
       </c>
       <c r="AT56" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="57">
@@ -8283,31 +8283,31 @@
         <v>1.0</v>
       </c>
       <c r="AL57" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AM57" s="1">
         <v>1.0</v>
       </c>
       <c r="AN57" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AO57" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AP57" s="1">
         <v>1.0</v>
       </c>
       <c r="AQ57" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AR57" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AS57" s="1">
         <v>1.0</v>
       </c>
       <c r="AT57" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="58">
@@ -8423,31 +8423,31 @@
         <v>1.0</v>
       </c>
       <c r="AL58" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AM58" s="1">
         <v>1.0</v>
       </c>
       <c r="AN58" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AO58" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AP58" s="1">
         <v>1.0</v>
       </c>
       <c r="AQ58" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AR58" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AS58" s="1">
         <v>1.0</v>
       </c>
       <c r="AT58" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="59">
@@ -8563,31 +8563,31 @@
         <v>1.0</v>
       </c>
       <c r="AL59" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AM59" s="1">
         <v>1.0</v>
       </c>
       <c r="AN59" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AO59" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AP59" s="1">
         <v>1.0</v>
       </c>
       <c r="AQ59" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AR59" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AS59" s="1">
         <v>1.0</v>
       </c>
       <c r="AT59" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="60">
@@ -8703,31 +8703,31 @@
         <v>1.0</v>
       </c>
       <c r="AL60" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AM60" s="1">
         <v>1.0</v>
       </c>
       <c r="AN60" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AO60" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AP60" s="1">
         <v>1.0</v>
       </c>
       <c r="AQ60" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AR60" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AS60" s="1">
         <v>1.0</v>
       </c>
       <c r="AT60" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="61">
@@ -8843,31 +8843,31 @@
         <v>1.0</v>
       </c>
       <c r="AL61" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AM61" s="1">
         <v>1.0</v>
       </c>
       <c r="AN61" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AO61" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AP61" s="1">
         <v>1.0</v>
       </c>
       <c r="AQ61" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AR61" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AS61" s="1">
         <v>1.0</v>
       </c>
       <c r="AT61" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="62">
@@ -8983,31 +8983,31 @@
         <v>1.0</v>
       </c>
       <c r="AL62" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AM62" s="1">
         <v>1.0</v>
       </c>
       <c r="AN62" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AO62" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AP62" s="1">
         <v>1.0</v>
       </c>
       <c r="AQ62" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AR62" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AS62" s="1">
         <v>1.0</v>
       </c>
       <c r="AT62" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="63">
@@ -9123,31 +9123,31 @@
         <v>1.0</v>
       </c>
       <c r="AL63" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AM63" s="1">
         <v>1.0</v>
       </c>
       <c r="AN63" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AO63" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AP63" s="1">
         <v>1.0</v>
       </c>
       <c r="AQ63" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AR63" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AS63" s="1">
         <v>1.0</v>
       </c>
       <c r="AT63" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="64">
@@ -9263,31 +9263,31 @@
         <v>1.0</v>
       </c>
       <c r="AL64" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AM64" s="1">
         <v>1.0</v>
       </c>
       <c r="AN64" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AO64" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AP64" s="1">
         <v>1.0</v>
       </c>
       <c r="AQ64" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AR64" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AS64" s="1">
         <v>1.0</v>
       </c>
       <c r="AT64" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="65">
@@ -9403,31 +9403,31 @@
         <v>1.0</v>
       </c>
       <c r="AL65" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AM65" s="1">
         <v>1.0</v>
       </c>
       <c r="AN65" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AO65" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AP65" s="1">
         <v>1.0</v>
       </c>
       <c r="AQ65" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AR65" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AS65" s="1">
         <v>1.0</v>
       </c>
       <c r="AT65" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="66">
@@ -9543,31 +9543,31 @@
         <v>1.0</v>
       </c>
       <c r="AL66" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AM66" s="1">
         <v>1.0</v>
       </c>
       <c r="AN66" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AO66" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AP66" s="1">
         <v>1.0</v>
       </c>
       <c r="AQ66" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AR66" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AS66" s="1">
         <v>1.0</v>
       </c>
       <c r="AT66" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="67">
@@ -9683,31 +9683,31 @@
         <v>1.0</v>
       </c>
       <c r="AL67" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AM67" s="1">
         <v>1.0</v>
       </c>
       <c r="AN67" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AO67" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AP67" s="1">
         <v>1.0</v>
       </c>
       <c r="AQ67" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AR67" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AS67" s="1">
         <v>1.0</v>
       </c>
       <c r="AT67" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="68">
@@ -9823,31 +9823,31 @@
         <v>1.0</v>
       </c>
       <c r="AL68" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AM68" s="1">
         <v>1.0</v>
       </c>
       <c r="AN68" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AO68" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AP68" s="1">
         <v>1.0</v>
       </c>
       <c r="AQ68" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AR68" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AS68" s="1">
         <v>1.0</v>
       </c>
       <c r="AT68" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="69">
@@ -9963,31 +9963,31 @@
         <v>1.0</v>
       </c>
       <c r="AL69" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AM69" s="1">
         <v>1.0</v>
       </c>
       <c r="AN69" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AO69" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AP69" s="1">
         <v>1.0</v>
       </c>
       <c r="AQ69" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AR69" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AS69" s="1">
         <v>1.0</v>
       </c>
       <c r="AT69" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="70">
@@ -10103,31 +10103,31 @@
         <v>1.0</v>
       </c>
       <c r="AL70" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AM70" s="1">
         <v>1.0</v>
       </c>
       <c r="AN70" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AO70" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AP70" s="1">
         <v>1.0</v>
       </c>
       <c r="AQ70" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AR70" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AS70" s="1">
         <v>1.0</v>
       </c>
       <c r="AT70" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="71">
@@ -10243,31 +10243,31 @@
         <v>1.0</v>
       </c>
       <c r="AL71" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AM71" s="1">
         <v>1.0</v>
       </c>
       <c r="AN71" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AO71" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AP71" s="1">
         <v>1.0</v>
       </c>
       <c r="AQ71" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AR71" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AS71" s="1">
         <v>1.0</v>
       </c>
       <c r="AT71" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="72">
@@ -10383,31 +10383,31 @@
         <v>1.0</v>
       </c>
       <c r="AL72" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AM72" s="1">
         <v>1.0</v>
       </c>
       <c r="AN72" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AO72" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AP72" s="1">
         <v>1.0</v>
       </c>
       <c r="AQ72" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AR72" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AS72" s="1">
         <v>1.0</v>
       </c>
       <c r="AT72" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="73">
@@ -10523,31 +10523,31 @@
         <v>1.0</v>
       </c>
       <c r="AL73" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AM73" s="1">
         <v>1.0</v>
       </c>
       <c r="AN73" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AO73" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AP73" s="1">
         <v>1.0</v>
       </c>
       <c r="AQ73" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AR73" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AS73" s="1">
         <v>1.0</v>
       </c>
       <c r="AT73" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="74">
@@ -10663,31 +10663,31 @@
         <v>1.0</v>
       </c>
       <c r="AL74" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AM74" s="1">
         <v>1.0</v>
       </c>
       <c r="AN74" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AO74" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AP74" s="1">
         <v>1.0</v>
       </c>
       <c r="AQ74" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AR74" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AS74" s="1">
         <v>1.0</v>
       </c>
       <c r="AT74" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="75">
@@ -10803,31 +10803,31 @@
         <v>1.0</v>
       </c>
       <c r="AL75" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AM75" s="1">
         <v>1.0</v>
       </c>
       <c r="AN75" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AO75" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AP75" s="1">
         <v>1.0</v>
       </c>
       <c r="AQ75" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AR75" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AS75" s="1">
         <v>1.0</v>
       </c>
       <c r="AT75" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="76">
@@ -10943,31 +10943,31 @@
         <v>1.0</v>
       </c>
       <c r="AL76" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AM76" s="1">
         <v>1.0</v>
       </c>
       <c r="AN76" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AO76" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AP76" s="1">
         <v>1.0</v>
       </c>
       <c r="AQ76" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AR76" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AS76" s="1">
         <v>1.0</v>
       </c>
       <c r="AT76" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="77">
@@ -11083,31 +11083,31 @@
         <v>1.0</v>
       </c>
       <c r="AL77" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AM77" s="1">
         <v>1.0</v>
       </c>
       <c r="AN77" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AO77" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AP77" s="1">
         <v>1.0</v>
       </c>
       <c r="AQ77" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AR77" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AS77" s="1">
         <v>1.0</v>
       </c>
       <c r="AT77" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="78">
@@ -11223,31 +11223,31 @@
         <v>1.0</v>
       </c>
       <c r="AL78" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AM78" s="1">
         <v>1.0</v>
       </c>
       <c r="AN78" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AO78" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AP78" s="1">
         <v>1.0</v>
       </c>
       <c r="AQ78" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AR78" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AS78" s="1">
         <v>1.0</v>
       </c>
       <c r="AT78" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="79">
@@ -11363,31 +11363,31 @@
         <v>1.0</v>
       </c>
       <c r="AL79" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AM79" s="1">
         <v>1.0</v>
       </c>
       <c r="AN79" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AO79" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AP79" s="1">
         <v>1.0</v>
       </c>
       <c r="AQ79" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AR79" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AS79" s="1">
         <v>1.0</v>
       </c>
       <c r="AT79" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="80">
@@ -11503,31 +11503,31 @@
         <v>1.0</v>
       </c>
       <c r="AL80" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AM80" s="1">
         <v>1.0</v>
       </c>
       <c r="AN80" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AO80" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AP80" s="1">
         <v>1.0</v>
       </c>
       <c r="AQ80" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AR80" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AS80" s="1">
         <v>1.0</v>
       </c>
       <c r="AT80" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="81">
@@ -11643,31 +11643,31 @@
         <v>1.0</v>
       </c>
       <c r="AL81" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AM81" s="1">
         <v>1.0</v>
       </c>
       <c r="AN81" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AO81" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AP81" s="1">
         <v>1.0</v>
       </c>
       <c r="AQ81" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AR81" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AS81" s="1">
         <v>1.0</v>
       </c>
       <c r="AT81" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="82">
@@ -11783,31 +11783,31 @@
         <v>1.0</v>
       </c>
       <c r="AL82" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AM82" s="1">
         <v>1.0</v>
       </c>
       <c r="AN82" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AO82" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AP82" s="1">
         <v>1.0</v>
       </c>
       <c r="AQ82" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AR82" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AS82" s="1">
         <v>1.0</v>
       </c>
       <c r="AT82" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="83">
@@ -11923,31 +11923,31 @@
         <v>1.0</v>
       </c>
       <c r="AL83" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AM83" s="1">
         <v>1.0</v>
       </c>
       <c r="AN83" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AO83" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AP83" s="1">
         <v>1.0</v>
       </c>
       <c r="AQ83" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AR83" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AS83" s="1">
         <v>1.0</v>
       </c>
       <c r="AT83" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="84">
@@ -12063,31 +12063,31 @@
         <v>1.0</v>
       </c>
       <c r="AL84" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AM84" s="1">
         <v>1.0</v>
       </c>
       <c r="AN84" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AO84" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AP84" s="1">
         <v>1.0</v>
       </c>
       <c r="AQ84" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AR84" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AS84" s="1">
         <v>1.0</v>
       </c>
       <c r="AT84" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="85">
@@ -12203,31 +12203,31 @@
         <v>1.0</v>
       </c>
       <c r="AL85" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AM85" s="1">
         <v>1.0</v>
       </c>
       <c r="AN85" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AO85" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AP85" s="1">
         <v>1.0</v>
       </c>
       <c r="AQ85" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AR85" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AS85" s="1">
         <v>1.0</v>
       </c>
       <c r="AT85" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="86">
@@ -12343,31 +12343,31 @@
         <v>1.0</v>
       </c>
       <c r="AL86" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AM86" s="1">
         <v>1.0</v>
       </c>
       <c r="AN86" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AO86" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AP86" s="1">
         <v>1.0</v>
       </c>
       <c r="AQ86" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AR86" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AS86" s="1">
         <v>1.0</v>
       </c>
       <c r="AT86" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="87">
@@ -12483,31 +12483,31 @@
         <v>1.0</v>
       </c>
       <c r="AL87" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AM87" s="1">
         <v>1.0</v>
       </c>
       <c r="AN87" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AO87" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AP87" s="1">
         <v>1.0</v>
       </c>
       <c r="AQ87" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AR87" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AS87" s="1">
         <v>1.0</v>
       </c>
       <c r="AT87" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="88">
@@ -12623,31 +12623,31 @@
         <v>1.0</v>
       </c>
       <c r="AL88" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AM88" s="1">
         <v>1.0</v>
       </c>
       <c r="AN88" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AO88" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AP88" s="1">
         <v>1.0</v>
       </c>
       <c r="AQ88" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AR88" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AS88" s="1">
         <v>1.0</v>
       </c>
       <c r="AT88" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="89">
@@ -12763,31 +12763,31 @@
         <v>1.0</v>
       </c>
       <c r="AL89" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AM89" s="1">
         <v>1.0</v>
       </c>
       <c r="AN89" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AO89" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AP89" s="1">
         <v>1.0</v>
       </c>
       <c r="AQ89" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AR89" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AS89" s="1">
         <v>1.0</v>
       </c>
       <c r="AT89" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="90">
@@ -12903,31 +12903,31 @@
         <v>1.0</v>
       </c>
       <c r="AL90" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AM90" s="1">
         <v>1.0</v>
       </c>
       <c r="AN90" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AO90" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AP90" s="1">
         <v>1.0</v>
       </c>
       <c r="AQ90" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AR90" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AS90" s="1">
         <v>1.0</v>
       </c>
       <c r="AT90" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="91">
@@ -13043,31 +13043,31 @@
         <v>1.0</v>
       </c>
       <c r="AL91" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AM91" s="1">
         <v>1.0</v>
       </c>
       <c r="AN91" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AO91" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AP91" s="1">
         <v>1.0</v>
       </c>
       <c r="AQ91" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AR91" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AS91" s="1">
         <v>1.0</v>
       </c>
       <c r="AT91" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="92">
@@ -13183,31 +13183,31 @@
         <v>1.0</v>
       </c>
       <c r="AL92" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AM92" s="1">
         <v>1.0</v>
       </c>
       <c r="AN92" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AO92" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AP92" s="1">
         <v>1.0</v>
       </c>
       <c r="AQ92" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AR92" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AS92" s="1">
         <v>1.0</v>
       </c>
       <c r="AT92" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="93">
@@ -13323,31 +13323,31 @@
         <v>1.0</v>
       </c>
       <c r="AL93" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AM93" s="1">
         <v>1.0</v>
       </c>
       <c r="AN93" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AO93" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AP93" s="1">
         <v>1.0</v>
       </c>
       <c r="AQ93" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AR93" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AS93" s="1">
         <v>1.0</v>
       </c>
       <c r="AT93" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="94">
@@ -13463,31 +13463,31 @@
         <v>1.0</v>
       </c>
       <c r="AL94" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AM94" s="1">
         <v>1.0</v>
       </c>
       <c r="AN94" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AO94" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AP94" s="1">
         <v>1.0</v>
       </c>
       <c r="AQ94" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AR94" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AS94" s="1">
         <v>1.0</v>
       </c>
       <c r="AT94" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="95">
@@ -13603,31 +13603,31 @@
         <v>1.0</v>
       </c>
       <c r="AL95" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AM95" s="1">
         <v>1.0</v>
       </c>
       <c r="AN95" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AO95" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AP95" s="1">
         <v>1.0</v>
       </c>
       <c r="AQ95" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AR95" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AS95" s="1">
         <v>1.0</v>
       </c>
       <c r="AT95" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="96">
@@ -13743,31 +13743,31 @@
         <v>1.0</v>
       </c>
       <c r="AL96" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AM96" s="1">
         <v>1.0</v>
       </c>
       <c r="AN96" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AO96" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AP96" s="1">
         <v>1.0</v>
       </c>
       <c r="AQ96" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AR96" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AS96" s="1">
         <v>1.0</v>
       </c>
       <c r="AT96" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="97">
@@ -13883,31 +13883,31 @@
         <v>1.0</v>
       </c>
       <c r="AL97" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AM97" s="1">
         <v>1.0</v>
       </c>
       <c r="AN97" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AO97" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AP97" s="1">
         <v>1.0</v>
       </c>
       <c r="AQ97" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AR97" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AS97" s="1">
         <v>1.0</v>
       </c>
       <c r="AT97" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="98">
@@ -14023,31 +14023,31 @@
         <v>1.0</v>
       </c>
       <c r="AL98" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AM98" s="1">
         <v>1.0</v>
       </c>
       <c r="AN98" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AO98" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AP98" s="1">
         <v>1.0</v>
       </c>
       <c r="AQ98" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AR98" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AS98" s="1">
         <v>1.0</v>
       </c>
       <c r="AT98" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="99">
@@ -14163,31 +14163,31 @@
         <v>1.0</v>
       </c>
       <c r="AL99" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AM99" s="1">
         <v>1.0</v>
       </c>
       <c r="AN99" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AO99" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AP99" s="1">
         <v>1.0</v>
       </c>
       <c r="AQ99" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AR99" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AS99" s="1">
         <v>1.0</v>
       </c>
       <c r="AT99" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="100">
@@ -14303,31 +14303,31 @@
         <v>1.0</v>
       </c>
       <c r="AL100" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AM100" s="1">
         <v>1.0</v>
       </c>
       <c r="AN100" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AO100" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AP100" s="1">
         <v>1.0</v>
       </c>
       <c r="AQ100" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AR100" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AS100" s="1">
         <v>1.0</v>
       </c>
       <c r="AT100" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="101">

</xml_diff>